<commit_message>
created test cases for api_signup_password_field and executed api_signup_username and symlex_portocol_settings
</commit_message>
<xml_diff>
--- a/api/app_api/backlog/signup/username_field.xlsx
+++ b/api/app_api/backlog/signup/username_field.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\api\app_api\backlog\signup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E1E5D3-3DE2-4F93-B374-B8F2E1AC7B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A80380-A996-4455-9327-59E81E7B6785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="129">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>verify username field with duplicate value already existing in the database</t>
-  </si>
-  <si>
-    <t>should return an error response with status code 409</t>
   </si>
   <si>
     <t>1. open the postman
@@ -465,6 +462,132 @@
 5. send the request with valid username but invalid password
 6. review the response status code.</t>
   </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>SYM-API-SP-029</t>
+  </si>
+  <si>
+    <t>test username field with valid email format</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST - User Signup)
+4. fill the other required field with valid credentials and goto username field
+5. send the request with valid email format
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> post request should return a successful response with status code 200</t>
+  </si>
+  <si>
+    <t>should return a successful response with status code 200
+(actual result : 422 status code)</t>
+  </si>
+  <si>
+    <t>post request should return a successful response with status code 200
+(actual result: 422 status code)</t>
+  </si>
+  <si>
+    <t>should return an error response with status code 409
+(actual result: 422 status code)</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>test username field with invalid email format</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST - User Signup)
+4. fill the other required field with valid credentials and goto username field
+5. send the request with invalid email format
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> post request should return a successful response with status code 400</t>
+  </si>
+  <si>
+    <t>SYM-API-SP-030</t>
+  </si>
+  <si>
+    <t>SYM-API-SP-031</t>
+  </si>
+  <si>
+    <t>SYM-API-SP-032</t>
+  </si>
+  <si>
+    <t>SYM-API-SP-033</t>
+  </si>
+  <si>
+    <t>SYM-API-SP-034</t>
+  </si>
+  <si>
+    <t>SYM-API-SP-035</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST - User Signup)
+4. fill the other required field with valid credentials and goto username field
+5. send the request with invalid email format containing an underscore
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> post request should return an error response with status code 400</t>
+  </si>
+  <si>
+    <t>verify input with invalid email format containing an underscore</t>
+  </si>
+  <si>
+    <t>verify input with invalid email format containing consecutive hyphens</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST - User Signup)
+4. fill the other required field with valid credentials and goto username field
+5. send the request with invalid email format containing consecutive hyphens
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>input with invalid email format containing an invalid character in the local part</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST - User Signup)
+4. fill the other required field with valid credentials and goto username field
+5. send the request with invalid email format containing an invalid character in the local part
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>verify input with invalid email format containing 
+an incomplete top-level domain</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST - User Signup)
+4. fill the other required field with valid credentials and goto username field
+5. send the request with invalid email format containing an incomplete top-level domain
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>input with invalid email format containing an incomplete local part</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST - User Signup)
+4. fill the other required field with valid credentials and goto username field
+5. send the request with invalid email format containing an incomplete local part
+6. review the response status code.</t>
+  </si>
 </sst>
 </file>
 
@@ -516,7 +639,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -539,6 +662,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
         <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -657,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -718,6 +859,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,7 +922,9 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -931,9 +1086,11 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -946,6 +1103,8 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -960,7 +1119,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1635,8 +1793,8 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" totalsRowLabel="verify username field with empty value" dataDxfId="11" totalsRowDxfId="4"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" totalsRowLabel="1. open the postman_x000a_2. create or open the saved request_x000a_3. define request(method -POST - User Signup)_x000a_4. fill the other required field with valid credentials and goto username field_x000a_5. send the request with empty value_x000a_6. review the response status code." dataDxfId="10" totalsRowDxfId="3"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" totalsRowLabel="post request should return an error response with status code 400" dataDxfId="9" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" totalsRowLabel="N/A" dataDxfId="8" totalsRowDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="7" totalsRowDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" totalsRowLabel="Pass" dataDxfId="7" totalsRowDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="8" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Template-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1843,11 +2001,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Z990"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1857,7 +2015,7 @@
     <col min="3" max="3" width="45.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" customWidth="1"/>
     <col min="5" max="5" width="45.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
     <col min="7" max="7" width="40.7109375" customWidth="1"/>
     <col min="8" max="16" width="14.42578125" customWidth="1"/>
   </cols>
@@ -1973,13 +2131,13 @@
         <v>32</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>8</v>
@@ -2015,13 +2173,13 @@
         <v>33</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="3"/>
@@ -2051,14 +2209,14 @@
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="22" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>7</v>
@@ -2095,13 +2253,13 @@
         <v>36</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>7</v>
+      <c r="F7" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="3"/>
@@ -2135,13 +2293,13 @@
         <v>38</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -2175,13 +2333,13 @@
         <v>40</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="5"/>
@@ -2211,14 +2369,14 @@
       <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="22" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>7</v>
@@ -2251,14 +2409,14 @@
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="23" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>7</v>
@@ -2292,16 +2450,16 @@
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -2332,16 +2490,16 @@
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
@@ -2372,16 +2530,16 @@
         <v>9</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
@@ -2412,16 +2570,16 @@
         <v>9</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="1"/>
@@ -2452,16 +2610,16 @@
         <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="1"/>
@@ -2492,16 +2650,16 @@
         <v>9</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="1"/>
@@ -2532,16 +2690,16 @@
         <v>9</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="1"/>
@@ -2572,16 +2730,16 @@
         <v>9</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="1"/>
@@ -2612,16 +2770,16 @@
         <v>9</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="1"/>
@@ -2651,11 +2809,11 @@
       <c r="B21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>71</v>
+      <c r="C21" s="23" t="s">
+        <v>70</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>34</v>
@@ -2691,11 +2849,11 @@
       <c r="B22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>73</v>
+      <c r="C22" s="23" t="s">
+        <v>72</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>37</v>
@@ -2732,16 +2890,16 @@
         <v>9</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="1"/>
@@ -2766,22 +2924,22 @@
     </row>
     <row r="24" spans="1:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>78</v>
+      <c r="C24" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>7</v>
+      <c r="F24" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="1"/>
@@ -2806,22 +2964,22 @@
     </row>
     <row r="25" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>80</v>
+      <c r="C25" s="23" t="s">
+        <v>79</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>7</v>
+      <c r="F25" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="1"/>
@@ -2846,22 +3004,22 @@
     </row>
     <row r="26" spans="1:26" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>7</v>
+      <c r="F26" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="1"/>
@@ -2886,22 +3044,22 @@
     </row>
     <row r="27" spans="1:26" ht="129" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>7</v>
+      <c r="F27" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="1"/>
@@ -2926,22 +3084,22 @@
     </row>
     <row r="28" spans="1:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>7</v>
+      <c r="F28" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="1"/>
@@ -2966,21 +3124,21 @@
     </row>
     <row r="29" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>95</v>
+      <c r="C29" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="9" t="s">
         <v>7</v>
       </c>
       <c r="G29" s="6"/>
@@ -3006,22 +3164,22 @@
     </row>
     <row r="30" spans="1:26" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>7</v>
+      <c r="F30" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="1"/>
@@ -3046,22 +3204,22 @@
     </row>
     <row r="31" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>7</v>
+      <c r="F31" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="1"/>
@@ -3084,13 +3242,25 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+    <row r="32" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="G32" s="6"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -3112,13 +3282,25 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
+    <row r="33" spans="1:26" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="G33" s="6"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -3140,13 +3322,25 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+    <row r="34" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G34" s="6"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -3168,13 +3362,25 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
+    <row r="35" spans="1:26" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G35" s="6"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -3196,13 +3402,25 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
+    <row r="36" spans="1:26" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G36" s="6"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -3224,13 +3442,25 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
+    <row r="37" spans="1:26" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G37" s="6"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -3252,13 +3482,25 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
+    <row r="38" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="G38" s="6"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -3281,12 +3523,12 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="9"/>
       <c r="G39" s="6"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -3309,12 +3551,12 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="9"/>
       <c r="G40" s="6"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -3337,12 +3579,12 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="9"/>
       <c r="G41" s="6"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -3365,12 +3607,12 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="9"/>
       <c r="G42" s="6"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -3393,12 +3635,12 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="9"/>
       <c r="G43" s="6"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -3421,12 +3663,12 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="9"/>
       <c r="G44" s="6"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -3449,12 +3691,12 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="9"/>
       <c r="G45" s="6"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -3477,12 +3719,12 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="9"/>
       <c r="G46" s="6"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -3505,12 +3747,12 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="9"/>
       <c r="G47" s="6"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -3533,12 +3775,12 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="9"/>
       <c r="G48" s="6"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -3561,12 +3803,12 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="9"/>
       <c r="G49" s="6"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -3589,12 +3831,12 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="9"/>
       <c r="G50" s="6"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -3617,12 +3859,12 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="9"/>
       <c r="G51" s="6"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -3645,12 +3887,12 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="9"/>
       <c r="G52" s="6"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -3673,12 +3915,12 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
+      <c r="A53" s="8"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="9"/>
       <c r="G53" s="6"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -3701,12 +3943,12 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="9"/>
       <c r="G54" s="6"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -3729,12 +3971,12 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="9"/>
       <c r="G55" s="6"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -29825,13 +30067,6 @@
       <c r="Z986" s="1"/>
     </row>
     <row r="987" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A987" s="6"/>
-      <c r="B987" s="6"/>
-      <c r="C987" s="6"/>
-      <c r="D987" s="6"/>
-      <c r="E987" s="6"/>
-      <c r="F987" s="6"/>
-      <c r="G987" s="6"/>
       <c r="H987" s="1"/>
       <c r="I987" s="1"/>
       <c r="J987" s="1"/>
@@ -29853,13 +30088,6 @@
       <c r="Z987" s="1"/>
     </row>
     <row r="988" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A988" s="6"/>
-      <c r="B988" s="6"/>
-      <c r="C988" s="6"/>
-      <c r="D988" s="6"/>
-      <c r="E988" s="6"/>
-      <c r="F988" s="6"/>
-      <c r="G988" s="6"/>
       <c r="H988" s="1"/>
       <c r="I988" s="1"/>
       <c r="J988" s="1"/>
@@ -29880,54 +30108,12 @@
       <c r="Y988" s="1"/>
       <c r="Z988" s="1"/>
     </row>
-    <row r="989" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H989" s="1"/>
-      <c r="I989" s="1"/>
-      <c r="J989" s="1"/>
-      <c r="K989" s="1"/>
-      <c r="L989" s="1"/>
-      <c r="M989" s="1"/>
-      <c r="N989" s="1"/>
-      <c r="O989" s="1"/>
-      <c r="P989" s="1"/>
-      <c r="Q989" s="1"/>
-      <c r="R989" s="1"/>
-      <c r="S989" s="1"/>
-      <c r="T989" s="1"/>
-      <c r="U989" s="1"/>
-      <c r="V989" s="1"/>
-      <c r="W989" s="1"/>
-      <c r="X989" s="1"/>
-      <c r="Y989" s="1"/>
-      <c r="Z989" s="1"/>
-    </row>
-    <row r="990" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H990" s="1"/>
-      <c r="I990" s="1"/>
-      <c r="J990" s="1"/>
-      <c r="K990" s="1"/>
-      <c r="L990" s="1"/>
-      <c r="M990" s="1"/>
-      <c r="N990" s="1"/>
-      <c r="O990" s="1"/>
-      <c r="P990" s="1"/>
-      <c r="Q990" s="1"/>
-      <c r="R990" s="1"/>
-      <c r="S990" s="1"/>
-      <c r="T990" s="1"/>
-      <c r="U990" s="1"/>
-      <c r="V990" s="1"/>
-      <c r="W990" s="1"/>
-      <c r="X990" s="1"/>
-      <c r="Y990" s="1"/>
-      <c r="Z990" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F6 F8:F31" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F55" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>